<commit_message>
Data preprocessing - Removal of names
</commit_message>
<xml_diff>
--- a/AzureOpenAIChatGTPAutoGrader-main/Assessment_Feedback.xlsx
+++ b/AzureOpenAIChatGTPAutoGrader-main/Assessment_Feedback.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Copy of FYP UP2061187 2.pdf</t>
+          <t>Copy of FYP UP2061187.pdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,40 +468,11 @@
   "Structure and presentation.": 60,
   "Overall understanding and reflection.": 40,
   "Final Mark": 30,
-  "Comments": "Overall, your project has some strong points but also some areas for improvement. Your statement of project's context, aims, and objectives is well presented and shows a clear understanding of the problem. The critical review of relevant literature is comprehensive, and you provide a good overview of the existing research. However, there is no discussion of the methodological approach, specification and discussion of the requirements, evaluation against requirements, evidence of project planning and management, or attributes of the solution. It is important to address these areas in order to provide a complete and well-rounded project. The analysis and discussion of the IT design is sufficient, but it would benefit from more detail and justification of design decisions. The discussion of implementation lacks specific details and justification. The discussion of verification and validation is strong and provides a good overall understanding. The summary, conclusions, and recommendations are well-written and offer valuable insights. The structure and presentation of the report is good, with clear headings and organization. However, there are some minor issues with grammar and punctuation that can be improved. Your overall understanding and reflection of the project is satisfactory, but there is room for deeper analysis and critical thinking. Based on these observations, your final mark is 30. Keep up the good work and consider addressing the areas for improvement in future projects."
-}</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Copy of FYP UP2061187.pdf</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>{
-  "Statement of project’s context, aims and objectives.": 75,
-  "Critical review of relevant literature.": 70,
-  "Methodological approach.": 0,
-  "Specification and discussion of the requirements.": 0,
-  "Analysis and discussion of the IT design.": 50,
-  "Discussion of implementation.": 40,
-  "Discussion of verification and validation.": 60,
-  "Evaluation against requirements.": 0,
-  "Evidence of project planning and management.": 0,
-  "Attributes of the solution.": 0,
-  "Summary, conclusions and recommendations.": 50,
-  "Structure and presentation.": 60,
-  "Overall understanding and reflection.": 40,
-  "Final Mark": 30,
-  "Comments": "Thank you for sharing your final year project with me. I appreciate the effort you put into researching and presenting your work. Your statement of the project's context, aims, and objectives is well-framed and demonstrates a clear understanding of the problem. Your critical review of the literature is comprehensive and shows a good understanding of the relevant research in the field.
-However, there are some areas where improvements can be made. The methodological approach is not discussed in your report, reducing the overall score in that category. Similarly, the specification and discussion of requirements are missing, which affects the score for that criteria. I encourage you to provide more detailed descriptions and justifications for the methods and requirements used in your project.
-The analysis and discussion of the IT design could be more thorough, providing a deeper understanding of the solution's architecture and design choices. Additionally, the discussion of implementation should be more comprehensive, covering the decisions made and trade-offs considered.
-While there is no evidence of project planning and management mentioned in the report, it would be beneficial to include details of your project plan, time-scales, resources, and any deviations from the plan. This would demonstrate your ability to effectively manage the project.
-The attributes of the solution category received a score of 0 as no evaluation or demonstration of the solution was provided in the report.
-In conclusion, your report shows promise, but there are areas for improvement. I encourage you to further develop your understanding of the project's methodology, requirements, design, and implementation. It is crucial to provide evidence of project planning and management, as well as an evaluation of the solution. These improvements will help elevate your final mark. Keep up the good work and continue to seek feedback to enhance your skills and knowledge. Good luck with your future endeavors!"
+  "Comments": "Thank you for sharing your final-year project with me. It is evident that you have put in effort and thought into your work. Your statement of the project's context, aims, and objectives is well-presented and provides a clear understanding of the problem and your goals. Your critical review of relevant literature demonstrates your research skills and your ability to analyze existing works in the field. 
+However, there are areas for improvement. Your methodology, specification and discussion of the requirements, and evaluation against requirements sections are missing. It is important to clearly outline the methodology and specify the requirements to ensure a comprehensive and well-rounded project. Additionally, an evaluation against requirements allows for a clear understanding of the project's success in meeting its goals. I encourage you to include these sections in your future work.
+Your analysis and discussion of the IT design shows potential, but it would be beneficial to provide more in-depth analysis and justification for the design decisions. Similarly, your discussion of implementation should provide more detailed explanations and justifications for the decisions and trade-offs made.
+In terms of structure and presentation, your report is well-organized with clear headings and sections. The use of diagrams and tables adds to the clarity of your work. Keep up the good work in this area.
+Overall, it is evident that you have a good understanding of the subject matter and have made progress in your research and project development. I encourage you to address the areas for improvement mentioned above in order to strengthen your project further. Well done on your efforts thus far."
 }</t>
         </is>
       </c>

</xml_diff>